<commit_message>
Update Use cases with actors.xlsx
</commit_message>
<xml_diff>
--- a/Use cases with actors.xlsx
+++ b/Use cases with actors.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD12066-D240-45DB-9428-BDBC18856702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="27">
   <si>
     <t>Admin</t>
   </si>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +226,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -280,7 +287,7 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -313,6 +320,7 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="%40 - Vurgu3" xfId="5" builtinId="39"/>
@@ -602,26 +610,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="23.42578125" customWidth="1"/>
-    <col min="12" max="12" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
@@ -641,7 +649,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -654,12 +662,12 @@
       <c r="F2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="14"/>
       <c r="K2" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -677,7 +685,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -690,12 +698,12 @@
       <c r="F4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="14"/>
       <c r="K4" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -713,7 +721,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -728,7 +736,7 @@
       </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -741,9 +749,9 @@
       <c r="F7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -758,7 +766,7 @@
       </c>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -773,7 +781,7 @@
       </c>
       <c r="G9" s="8"/>
     </row>
-    <row r="10" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -788,7 +796,7 @@
       </c>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -803,7 +811,7 @@
       </c>
       <c r="G11" s="8"/>
     </row>
-    <row r="12" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -818,7 +826,7 @@
       </c>
       <c r="G12" s="8"/>
     </row>
-    <row r="13" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -833,7 +841,7 @@
       </c>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -846,9 +854,9 @@
       <c r="F14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -863,7 +871,7 @@
       </c>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -878,7 +886,7 @@
       </c>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -893,7 +901,7 @@
       </c>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
sequence finished for me
</commit_message>
<xml_diff>
--- a/Use cases with actors.xlsx
+++ b/Use cases with actors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>Admin</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Delete any Survey</t>
-  </si>
-  <si>
-    <t>Check all Survey Statistics</t>
   </si>
 </sst>
 </file>
@@ -615,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,21 +932,6 @@
       </c>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>